<commit_message>
Equal temp dep analysis and figs
</commit_message>
<xml_diff>
--- a/CODE/Data/Dc_cmax20-b250_D075_J100_A050_Sm025_nmort1_BE075_noCC_RE00100_Ka050/Hist_Fore_All_fish03_ensem6_mid_samek_prod_yield_diff_pdiff_MeanStd.xlsx
+++ b/CODE/Data/Dc_cmax20-b250_D075_J100_A050_Sm025_nmort1_BE075_noCC_RE00100_Ka050/Hist_Fore_All_fish03_ensem6_mid_samek_prod_yield_diff_pdiff_MeanStd.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpetrik/Dropbox/Princeton/FEISTY/CODE/Data/Dc_cmax20-b250_D075_J100_A050_Sm025_nmort1_BE075_noCC_RE00100_Ka050/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B9183948-EEF8-DD4C-A963-6CCC52D674D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7D5F8C-E468-3F48-AA2B-14B5B3F3DCCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="460" windowWidth="25200" windowHeight="17040"/>
+    <workbookView xWindow="1840" yWindow="460" windowWidth="25200" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hist_Fore_All_fish03_ensem6_mid" sheetId="1" r:id="rId1"/>
@@ -61,9 +61,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -577,22 +577,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="18" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -949,77 +949,77 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I8"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="3" width="9.83203125" customWidth="1"/>
-    <col min="4" max="9" width="9.33203125" customWidth="1"/>
+    <col min="4" max="9" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1033,22 +1033,22 @@
       <c r="C4" s="2">
         <v>143509191451.465</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>-6.5927886382873204</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>1.19325630072929</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>-2.32119294741327</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>0.58126996409075504</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>-9.7776302272016302</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>0.81897933611398599</v>
       </c>
     </row>
@@ -1062,22 +1062,22 @@
       <c r="C5" s="2">
         <v>153331654286.896</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>-11.062288390227501</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>3.00201255104861</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>-7.4224974783868101</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>1.18908130975296</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>-14.5312272494838</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>1.6611082521634799</v>
       </c>
     </row>
@@ -1091,22 +1091,22 @@
       <c r="C6" s="2">
         <v>11917080490.7269</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>-13.043031654023199</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>0.77942462530919399</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>-3.47771492225292</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>0.27761966888721301</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>-9.0838732453463802</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>0.42323367720796101</v>
       </c>
     </row>
@@ -1120,51 +1120,51 @@
       <c r="C7" s="2">
         <v>153869931764.08899</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>-8.5486065868783392</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>1.26950575239862</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>-13.221405348053</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>1.3070329632189499</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>-11.6353400797645</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>0.35591038698946798</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>-251709603916.01999</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>-12.296719262358501</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="7" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>